<commit_message>
several small fixes cleaning up sync log and one big one - TUC_EU-ElcTransCons-R and TUC_EU-ElcTransCons-NR
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SUBRES_20_TECHS_TRA_Trans.xlsx
+++ b/SubRES_TMPL/SUBRES_20_TECHS_TRA_Trans.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\EU-TIMES\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\EU_TIMES_Veda2p0\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A87995-820D-4B88-9C8C-B8809A87F2A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31FE40A-153D-4D2C-A1E3-B2C09CCAFC0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="570" windowWidth="25080" windowHeight="15030" tabRatio="909" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>